<commit_message>
Feature Add: Complete GUI along with functioning of the script.
</commit_message>
<xml_diff>
--- a/Main_extraction.xlsx
+++ b/Main_extraction.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,55 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Scrip_Symbol</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>B.Qty</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>B.Rate</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>S.Qty</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>S.Rate</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>N.Qty</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N.Rate</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>N.Amt</t>
         </is>
@@ -488,22 +493,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>BSE BSE - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>2024-06-28</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
@@ -514,34 +521,39 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>10</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>2598</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>-25979</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>544223 CEIGALL - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>2024-08-08</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
@@ -552,34 +564,39 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
         <v>37</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>401</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>-14837</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>544271 GARUDA - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>2025-01-27</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
@@ -590,34 +607,39 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>80</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>121</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>-9688</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>500116 IDBI - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>2024-07-23</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
@@ -628,34 +650,39 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>100</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>89</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>-8926</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>543398 LATENTVIEW - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>2025-01-08</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
@@ -666,34 +693,39 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
         <v>310</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>483</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>-149741</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>532461 PNB - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>2025-01-29</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
@@ -704,110 +736,125 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
         <v>935</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>98</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>-91705</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>532461 PNB - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Setl : M-2025613</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>265</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>103</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
         <v>265</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>103</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>-27261</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>532461 PNB - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>2025-05-07</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Setl : M-2025624</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>225</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>97</v>
       </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
         <v>225</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>97</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>-21812</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>544243 STYLEBAAZA - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>2024-09-05</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
@@ -818,34 +865,39 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>38</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>389</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>-14782</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>521064 TRIDENT - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>2024-07-31</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
@@ -856,34 +908,39 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
         <v>370</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>40</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>-14904</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BSE_CASH</t>
+          <t>543238 UTIAMC - MITHIL DEEPAK KOTWAL</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>BSE_CASH</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>2024-10-14</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>OPENING:CARRY FORWARD DATA FROM 2024</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
@@ -894,12 +951,15 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
         <v>171</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>1222</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>-208951</v>
       </c>
     </row>

</xml_diff>